<commit_message>
added results for Rust
</commit_message>
<xml_diff>
--- a/Benchmark/log_folder/benchmarking_version01.xlsx
+++ b/Benchmark/log_folder/benchmarking_version01.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ejer/Desktop/rustengine/Benchmark/log_folder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{29E58B76-1733-2F40-9950-FA5F76B76CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B430C1F-9815-3849-B049-A08FB9AF5DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16140" xr2:uid="{8B5CF308-BF6E-9F4F-9AA5-BFC8DF812455}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16140" activeTab="1" xr2:uid="{8B5CF308-BF6E-9F4F-9AA5-BFC8DF812455}"/>
   </bookViews>
   <sheets>
     <sheet name="results_c" sheetId="1" r:id="rId1"/>
+    <sheet name="results_rust" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="99">
   <si>
     <t xml:space="preserve">      Total Number of Cores: 4</t>
   </si>
@@ -200,6 +201,123 @@
   </si>
   <si>
     <t>199.89</t>
+  </si>
+  <si>
+    <t>./rustengine</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>0.14</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>13.54</t>
+  </si>
+  <si>
+    <t>0.47</t>
+  </si>
+  <si>
+    <t>13.53</t>
+  </si>
+  <si>
+    <t>0.48</t>
+  </si>
+  <si>
+    <t>13.55</t>
+  </si>
+  <si>
+    <t>13.56</t>
+  </si>
+  <si>
+    <t>14.27</t>
+  </si>
+  <si>
+    <t>13.78</t>
+  </si>
+  <si>
+    <t>13.98</t>
+  </si>
+  <si>
+    <t>13.50</t>
+  </si>
+  <si>
+    <t>0.46</t>
+  </si>
+  <si>
+    <t>13.58</t>
+  </si>
+  <si>
+    <t>140.45</t>
+  </si>
+  <si>
+    <t>135.49</t>
+  </si>
+  <si>
+    <t>140.10</t>
+  </si>
+  <si>
+    <t>135.25</t>
+  </si>
+  <si>
+    <t>142.90</t>
+  </si>
+  <si>
+    <t>137.53</t>
+  </si>
+  <si>
+    <t>143.75</t>
+  </si>
+  <si>
+    <t>138.17</t>
+  </si>
+  <si>
+    <t>142.94</t>
+  </si>
+  <si>
+    <t>137.59</t>
+  </si>
+  <si>
+    <t>141.02</t>
+  </si>
+  <si>
+    <t>136.00</t>
+  </si>
+  <si>
+    <t>151.78</t>
+  </si>
+  <si>
+    <t>144.50</t>
+  </si>
+  <si>
+    <t>146.57</t>
+  </si>
+  <si>
+    <t>140.09</t>
+  </si>
+  <si>
+    <t>146.83</t>
+  </si>
+  <si>
+    <t>140.79</t>
+  </si>
+  <si>
+    <t>140.55</t>
+  </si>
+  <si>
+    <t>135.60</t>
+  </si>
+  <si>
+    <t>140.25</t>
+  </si>
+  <si>
+    <t>135.36</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93E4383-DF91-4E42-A450-26BFB18058E7}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -3845,4 +3963,2798 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15423BDD-238C-304D-90DE-146BEECFB9AC}">
+  <dimension ref="A1:O68"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>45561.841631944444</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F3">
+        <v>728</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>407</v>
+      </c>
+      <c r="I3">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>45561.841631944444</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="F4">
+        <v>728</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>407</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>45561.841643518521</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F5">
+        <v>864</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>444</v>
+      </c>
+      <c r="I5">
+        <v>15</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
+        <v>60</v>
+      </c>
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>45561.841643518521</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="F6">
+        <v>728</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>407</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>45561.841643518521</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F7">
+        <v>728</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>408</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>45561.841643518521</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="F8">
+        <v>728</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>407</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>60</v>
+      </c>
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>45561.841643518521</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="F9">
+        <v>728</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>411</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>45561.841643518521</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="F10">
+        <v>728</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>404</v>
+      </c>
+      <c r="I10">
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>45561.841643518521</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F11">
+        <v>728</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>408</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
+        <v>60</v>
+      </c>
+      <c r="M11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>45561.841643518521</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F12">
+        <v>728</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>407</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" t="s">
+        <v>60</v>
+      </c>
+      <c r="M12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>45561.841643518521</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F13">
+        <v>728</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>404</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>60</v>
+      </c>
+      <c r="M13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="F14">
+        <v>928</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>457</v>
+      </c>
+      <c r="I14">
+        <v>17</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F15">
+        <v>896</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>449</v>
+      </c>
+      <c r="I15">
+        <v>29</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>10</v>
+      </c>
+      <c r="L15" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F16">
+        <v>844</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>441</v>
+      </c>
+      <c r="I16">
+        <v>17</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>10</v>
+      </c>
+      <c r="L16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F17">
+        <v>916</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>454</v>
+      </c>
+      <c r="I17">
+        <v>31</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>10</v>
+      </c>
+      <c r="L17" t="s">
+        <v>60</v>
+      </c>
+      <c r="M17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="F18">
+        <v>908</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>452</v>
+      </c>
+      <c r="I18">
+        <v>18</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+      <c r="L18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F19">
+        <v>728</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>407</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>10</v>
+      </c>
+      <c r="L19" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="F20">
+        <v>876</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>444</v>
+      </c>
+      <c r="I20">
+        <v>11</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>10</v>
+      </c>
+      <c r="L20" t="s">
+        <v>60</v>
+      </c>
+      <c r="M20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F21">
+        <v>880</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>445</v>
+      </c>
+      <c r="I21">
+        <v>12</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>10</v>
+      </c>
+      <c r="L21" t="s">
+        <v>60</v>
+      </c>
+      <c r="M21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.91</v>
+      </c>
+      <c r="F22">
+        <v>1000</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>475</v>
+      </c>
+      <c r="I22">
+        <v>45</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>10</v>
+      </c>
+      <c r="L22" t="s">
+        <v>60</v>
+      </c>
+      <c r="M22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F23">
+        <v>840</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>432</v>
+      </c>
+      <c r="I23">
+        <v>8</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>10</v>
+      </c>
+      <c r="L23" t="s">
+        <v>60</v>
+      </c>
+      <c r="M23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>45561.841747685183</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="F24">
+        <v>796</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>424</v>
+      </c>
+      <c r="I24">
+        <v>3</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>10</v>
+      </c>
+      <c r="L24" t="s">
+        <v>60</v>
+      </c>
+      <c r="M24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>45561.841863425929</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F25">
+        <v>1076</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>494</v>
+      </c>
+      <c r="I25">
+        <v>107</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>100</v>
+      </c>
+      <c r="L25" t="s">
+        <v>60</v>
+      </c>
+      <c r="M25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>45561.841863425929</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F26">
+        <v>1032</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>483</v>
+      </c>
+      <c r="I26">
+        <v>42</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>100</v>
+      </c>
+      <c r="L26" t="s">
+        <v>60</v>
+      </c>
+      <c r="M26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>45561.841863425929</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F27">
+        <v>916</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
+        <v>454</v>
+      </c>
+      <c r="I27">
+        <v>17</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>100</v>
+      </c>
+      <c r="L27" t="s">
+        <v>60</v>
+      </c>
+      <c r="M27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>45561.841863425929</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" t="s">
+        <v>62</v>
+      </c>
+      <c r="D28" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F28">
+        <v>1028</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>482</v>
+      </c>
+      <c r="I28">
+        <v>48</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>100</v>
+      </c>
+      <c r="L28" t="s">
+        <v>60</v>
+      </c>
+      <c r="M28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>45561.841874999998</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" t="s">
+        <v>63</v>
+      </c>
+      <c r="D29" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F29">
+        <v>864</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>441</v>
+      </c>
+      <c r="I29">
+        <v>14</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>100</v>
+      </c>
+      <c r="L29" t="s">
+        <v>60</v>
+      </c>
+      <c r="M29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>45561.841874999998</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F30">
+        <v>984</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>471</v>
+      </c>
+      <c r="I30">
+        <v>27</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>100</v>
+      </c>
+      <c r="L30" t="s">
+        <v>60</v>
+      </c>
+      <c r="M30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>45561.841874999998</v>
+      </c>
+      <c r="B31" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F31">
+        <v>964</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>466</v>
+      </c>
+      <c r="I31">
+        <v>16</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>100</v>
+      </c>
+      <c r="L31" t="s">
+        <v>60</v>
+      </c>
+      <c r="M31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>45561.841874999998</v>
+      </c>
+      <c r="B32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F32">
+        <v>900</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>450</v>
+      </c>
+      <c r="I32">
+        <v>17</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>100</v>
+      </c>
+      <c r="L32" t="s">
+        <v>60</v>
+      </c>
+      <c r="M32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>45561.841874999998</v>
+      </c>
+      <c r="B33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F33">
+        <v>1024</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>481</v>
+      </c>
+      <c r="I33">
+        <v>32</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>100</v>
+      </c>
+      <c r="L33" t="s">
+        <v>60</v>
+      </c>
+      <c r="M33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>45561.841874999998</v>
+      </c>
+      <c r="B34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D34" t="s">
+        <v>16</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="F34">
+        <v>916</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>454</v>
+      </c>
+      <c r="I34">
+        <v>14</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>100</v>
+      </c>
+      <c r="L34" t="s">
+        <v>60</v>
+      </c>
+      <c r="M34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>45561.841886574075</v>
+      </c>
+      <c r="B35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>62</v>
+      </c>
+      <c r="D35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F35">
+        <v>1004</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>476</v>
+      </c>
+      <c r="I35">
+        <v>33</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>100</v>
+      </c>
+      <c r="L35" t="s">
+        <v>60</v>
+      </c>
+      <c r="M35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>45561.842013888891</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1.42</v>
+      </c>
+      <c r="C36" s="3">
+        <v>13150</v>
+      </c>
+      <c r="D36" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F36">
+        <v>1060</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>490</v>
+      </c>
+      <c r="I36">
+        <v>226</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>1000</v>
+      </c>
+      <c r="L36" t="s">
+        <v>60</v>
+      </c>
+      <c r="M36" t="s">
+        <v>18</v>
+      </c>
+      <c r="O36" s="5"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>45561.842037037037</v>
+      </c>
+      <c r="B37" s="5">
+        <v>1.41</v>
+      </c>
+      <c r="C37" s="3">
+        <v>12785</v>
+      </c>
+      <c r="D37" t="s">
+        <v>64</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F37">
+        <v>996</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>474</v>
+      </c>
+      <c r="I37">
+        <v>109</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37">
+        <v>1000</v>
+      </c>
+      <c r="L37" t="s">
+        <v>60</v>
+      </c>
+      <c r="M37" t="s">
+        <v>18</v>
+      </c>
+      <c r="O37" s="5"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>45561.842048611114</v>
+      </c>
+      <c r="B38" s="5">
+        <v>1.43</v>
+      </c>
+      <c r="C38" s="3">
+        <v>13516</v>
+      </c>
+      <c r="D38" t="s">
+        <v>64</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F38">
+        <v>1132</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>508</v>
+      </c>
+      <c r="I38">
+        <v>295</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38">
+        <v>1000</v>
+      </c>
+      <c r="L38" t="s">
+        <v>60</v>
+      </c>
+      <c r="M38" t="s">
+        <v>18</v>
+      </c>
+      <c r="O38" s="5"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>45561.84207175926</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1.41</v>
+      </c>
+      <c r="C39" s="3">
+        <v>12785</v>
+      </c>
+      <c r="D39" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F39">
+        <v>1000</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>475</v>
+      </c>
+      <c r="I39">
+        <v>92</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39">
+        <v>1000</v>
+      </c>
+      <c r="L39" t="s">
+        <v>60</v>
+      </c>
+      <c r="M39" t="s">
+        <v>18</v>
+      </c>
+      <c r="O39" s="5"/>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>45561.842083333337</v>
+      </c>
+      <c r="B40" s="5">
+        <v>1.4</v>
+      </c>
+      <c r="C40" s="3">
+        <v>12785</v>
+      </c>
+      <c r="D40" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F40">
+        <v>1104</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>501</v>
+      </c>
+      <c r="I40">
+        <v>76</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>1000</v>
+      </c>
+      <c r="L40" t="s">
+        <v>60</v>
+      </c>
+      <c r="M40" t="s">
+        <v>18</v>
+      </c>
+      <c r="O40" s="5"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>45561.842106481483</v>
+      </c>
+      <c r="B41" s="6">
+        <v>1.41</v>
+      </c>
+      <c r="C41" s="3">
+        <v>12785</v>
+      </c>
+      <c r="D41" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F41">
+        <v>1004</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>476</v>
+      </c>
+      <c r="I41">
+        <v>132</v>
+      </c>
+      <c r="J41">
+        <v>0</v>
+      </c>
+      <c r="K41">
+        <v>1000</v>
+      </c>
+      <c r="L41" t="s">
+        <v>60</v>
+      </c>
+      <c r="M41" t="s">
+        <v>18</v>
+      </c>
+      <c r="O41" s="6"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>45561.842118055552</v>
+      </c>
+      <c r="B42" s="6">
+        <v>1.41</v>
+      </c>
+      <c r="C42" s="3">
+        <v>13150</v>
+      </c>
+      <c r="D42" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F42">
+        <v>1052</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>488</v>
+      </c>
+      <c r="I42">
+        <v>129</v>
+      </c>
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>1000</v>
+      </c>
+      <c r="L42" t="s">
+        <v>60</v>
+      </c>
+      <c r="M42" t="s">
+        <v>18</v>
+      </c>
+      <c r="O42" s="6"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>45561.842129629629</v>
+      </c>
+      <c r="B43" s="6">
+        <v>1.41</v>
+      </c>
+      <c r="C43" s="3">
+        <v>13150</v>
+      </c>
+      <c r="D43" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F43">
+        <v>1044</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>486</v>
+      </c>
+      <c r="I43">
+        <v>136</v>
+      </c>
+      <c r="J43">
+        <v>0</v>
+      </c>
+      <c r="K43">
+        <v>1000</v>
+      </c>
+      <c r="L43" t="s">
+        <v>60</v>
+      </c>
+      <c r="M43" t="s">
+        <v>18</v>
+      </c>
+      <c r="O43" s="6"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>45561.842152777775</v>
+      </c>
+      <c r="B44" s="6">
+        <v>1.41</v>
+      </c>
+      <c r="C44" s="3">
+        <v>12785</v>
+      </c>
+      <c r="D44" t="s">
+        <v>64</v>
+      </c>
+      <c r="E44" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F44">
+        <v>1012</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>478</v>
+      </c>
+      <c r="I44">
+        <v>111</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>1000</v>
+      </c>
+      <c r="L44" t="s">
+        <v>60</v>
+      </c>
+      <c r="M44" t="s">
+        <v>18</v>
+      </c>
+      <c r="O44" s="6"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>45561.842164351852</v>
+      </c>
+      <c r="B45" s="6">
+        <v>1.41</v>
+      </c>
+      <c r="C45" s="3">
+        <v>13150</v>
+      </c>
+      <c r="D45" t="s">
+        <v>64</v>
+      </c>
+      <c r="E45" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F45">
+        <v>1092</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>498</v>
+      </c>
+      <c r="I45">
+        <v>194</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>1000</v>
+      </c>
+      <c r="L45" t="s">
+        <v>60</v>
+      </c>
+      <c r="M45" t="s">
+        <v>18</v>
+      </c>
+      <c r="O45" s="6"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>45561.842187499999</v>
+      </c>
+      <c r="B46" s="6">
+        <v>1.41</v>
+      </c>
+      <c r="C46" s="3">
+        <v>12785</v>
+      </c>
+      <c r="D46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F46">
+        <v>1036</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>484</v>
+      </c>
+      <c r="I46">
+        <v>96</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>1000</v>
+      </c>
+      <c r="L46" t="s">
+        <v>60</v>
+      </c>
+      <c r="M46" t="s">
+        <v>18</v>
+      </c>
+      <c r="O46" s="6"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>45561.842314814814</v>
+      </c>
+      <c r="B47" s="5">
+        <v>14.03</v>
+      </c>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D47" t="s">
+        <v>66</v>
+      </c>
+      <c r="E47" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F47">
+        <v>1132</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>508</v>
+      </c>
+      <c r="I47">
+        <v>1190</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>10000</v>
+      </c>
+      <c r="L47" t="s">
+        <v>60</v>
+      </c>
+      <c r="M47" t="s">
+        <v>18</v>
+      </c>
+      <c r="O47" s="5"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>45561.842476851853</v>
+      </c>
+      <c r="B48" s="5">
+        <v>14.01</v>
+      </c>
+      <c r="C48" t="s">
+        <v>67</v>
+      </c>
+      <c r="D48" t="s">
+        <v>66</v>
+      </c>
+      <c r="E48" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F48">
+        <v>1112</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>503</v>
+      </c>
+      <c r="I48">
+        <v>982</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>10000</v>
+      </c>
+      <c r="L48" t="s">
+        <v>60</v>
+      </c>
+      <c r="M48" t="s">
+        <v>18</v>
+      </c>
+      <c r="O48" s="5"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>45561.842650462961</v>
+      </c>
+      <c r="B49" s="5">
+        <v>14.03</v>
+      </c>
+      <c r="C49" t="s">
+        <v>67</v>
+      </c>
+      <c r="D49" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F49">
+        <v>1132</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>508</v>
+      </c>
+      <c r="I49">
+        <v>1403</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>10000</v>
+      </c>
+      <c r="L49" t="s">
+        <v>60</v>
+      </c>
+      <c r="M49" t="s">
+        <v>18</v>
+      </c>
+      <c r="O49" s="5"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>45561.842812499999</v>
+      </c>
+      <c r="B50" s="5">
+        <v>14.04</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F50">
+        <v>1132</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>508</v>
+      </c>
+      <c r="I50">
+        <v>1569</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>10000</v>
+      </c>
+      <c r="L50" t="s">
+        <v>60</v>
+      </c>
+      <c r="M50" t="s">
+        <v>18</v>
+      </c>
+      <c r="O50" s="5"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>45561.842974537038</v>
+      </c>
+      <c r="B51" s="5">
+        <v>14.05</v>
+      </c>
+      <c r="C51" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" t="s">
+        <v>66</v>
+      </c>
+      <c r="E51" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F51">
+        <v>1132</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>508</v>
+      </c>
+      <c r="I51">
+        <v>1322</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>10000</v>
+      </c>
+      <c r="L51" t="s">
+        <v>60</v>
+      </c>
+      <c r="M51" t="s">
+        <v>18</v>
+      </c>
+      <c r="O51" s="5"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>45561.843136574076</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F52">
+        <v>1128</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>507</v>
+      </c>
+      <c r="I52">
+        <v>962</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>10000</v>
+      </c>
+      <c r="L52" t="s">
+        <v>60</v>
+      </c>
+      <c r="M52" t="s">
+        <v>18</v>
+      </c>
+      <c r="O52" s="5"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>45561.843298611115</v>
+      </c>
+      <c r="B53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C53" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" t="s">
+        <v>75</v>
+      </c>
+      <c r="E53" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F53">
+        <v>1120</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>505</v>
+      </c>
+      <c r="I53">
+        <v>1015</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>10000</v>
+      </c>
+      <c r="L53" t="s">
+        <v>60</v>
+      </c>
+      <c r="M53" t="s">
+        <v>18</v>
+      </c>
+      <c r="O53" s="5"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>45561.843460648146</v>
+      </c>
+      <c r="B54" s="5">
+        <v>14.08</v>
+      </c>
+      <c r="C54" t="s">
+        <v>76</v>
+      </c>
+      <c r="D54" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F54">
+        <v>1132</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54">
+        <v>508</v>
+      </c>
+      <c r="I54">
+        <v>1253</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>10000</v>
+      </c>
+      <c r="L54" t="s">
+        <v>60</v>
+      </c>
+      <c r="M54" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>45561.843622685185</v>
+      </c>
+      <c r="B55" s="5">
+        <v>14.03</v>
+      </c>
+      <c r="C55" t="s">
+        <v>67</v>
+      </c>
+      <c r="D55" t="s">
+        <v>68</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F55">
+        <v>1132</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>508</v>
+      </c>
+      <c r="I55">
+        <v>1283</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>10000</v>
+      </c>
+      <c r="L55" t="s">
+        <v>60</v>
+      </c>
+      <c r="M55" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>45561.843784722223</v>
+      </c>
+      <c r="B56" s="5">
+        <v>14.02</v>
+      </c>
+      <c r="C56" t="s">
+        <v>67</v>
+      </c>
+      <c r="D56" t="s">
+        <v>66</v>
+      </c>
+      <c r="E56" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F56">
+        <v>1132</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>508</v>
+      </c>
+      <c r="I56">
+        <v>1259</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>10000</v>
+      </c>
+      <c r="L56" t="s">
+        <v>60</v>
+      </c>
+      <c r="M56" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>45561.843946759262</v>
+      </c>
+      <c r="B57" t="s">
+        <v>73</v>
+      </c>
+      <c r="C57" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" t="s">
+        <v>75</v>
+      </c>
+      <c r="E57" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F57">
+        <v>1120</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>505</v>
+      </c>
+      <c r="I57">
+        <v>984</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>10000</v>
+      </c>
+      <c r="L57" t="s">
+        <v>60</v>
+      </c>
+      <c r="M57" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>45561.844351851854</v>
+      </c>
+      <c r="B58" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" t="s">
+        <v>78</v>
+      </c>
+      <c r="D58" s="3">
+        <v>29677</v>
+      </c>
+      <c r="E58" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F58">
+        <v>1132</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>508</v>
+      </c>
+      <c r="I58">
+        <v>13233</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>100000</v>
+      </c>
+      <c r="L58" t="s">
+        <v>60</v>
+      </c>
+      <c r="M58" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>45561.845983796295</v>
+      </c>
+      <c r="B59" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" s="3">
+        <v>26755</v>
+      </c>
+      <c r="E59" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F59">
+        <v>1120</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>505</v>
+      </c>
+      <c r="I59">
+        <v>11972</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>100000</v>
+      </c>
+      <c r="L59" t="s">
+        <v>60</v>
+      </c>
+      <c r="M59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>45561.847604166665</v>
+      </c>
+      <c r="B60" t="s">
+        <v>81</v>
+      </c>
+      <c r="C60" t="s">
+        <v>82</v>
+      </c>
+      <c r="D60" s="3">
+        <v>46143</v>
+      </c>
+      <c r="E60" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F60">
+        <v>1132</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>508</v>
+      </c>
+      <c r="I60">
+        <v>11868</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>100000</v>
+      </c>
+      <c r="L60" t="s">
+        <v>60</v>
+      </c>
+      <c r="M60" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>45561.849259259259</v>
+      </c>
+      <c r="B61" t="s">
+        <v>83</v>
+      </c>
+      <c r="C61" t="s">
+        <v>84</v>
+      </c>
+      <c r="D61" s="3">
+        <v>16193</v>
+      </c>
+      <c r="E61" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F61">
+        <v>1120</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>505</v>
+      </c>
+      <c r="I61">
+        <v>13376</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>100000</v>
+      </c>
+      <c r="L61" t="s">
+        <v>60</v>
+      </c>
+      <c r="M61" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>45561.850925925923</v>
+      </c>
+      <c r="B62" t="s">
+        <v>85</v>
+      </c>
+      <c r="C62" t="s">
+        <v>86</v>
+      </c>
+      <c r="D62" s="3">
+        <v>44682</v>
+      </c>
+      <c r="E62" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F62">
+        <v>1132</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>508</v>
+      </c>
+      <c r="I62">
+        <v>12253</v>
+      </c>
+      <c r="J62">
+        <v>0</v>
+      </c>
+      <c r="K62">
+        <v>100000</v>
+      </c>
+      <c r="L62" t="s">
+        <v>60</v>
+      </c>
+      <c r="M62" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>45561.852581018517</v>
+      </c>
+      <c r="B63" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" t="s">
+        <v>88</v>
+      </c>
+      <c r="D63" s="3">
+        <v>33329</v>
+      </c>
+      <c r="E63" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F63">
+        <v>1120</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>505</v>
+      </c>
+      <c r="I63">
+        <v>11393</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>100000</v>
+      </c>
+      <c r="L63" t="s">
+        <v>60</v>
+      </c>
+      <c r="M63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>45561.854212962964</v>
+      </c>
+      <c r="B64" t="s">
+        <v>89</v>
+      </c>
+      <c r="C64" t="s">
+        <v>90</v>
+      </c>
+      <c r="D64" s="3">
+        <v>30834</v>
+      </c>
+      <c r="E64" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F64">
+        <v>1132</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>508</v>
+      </c>
+      <c r="I64">
+        <v>27090</v>
+      </c>
+      <c r="J64">
+        <v>0</v>
+      </c>
+      <c r="K64">
+        <v>100000</v>
+      </c>
+      <c r="L64" t="s">
+        <v>60</v>
+      </c>
+      <c r="M64" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>45561.85596064815</v>
+      </c>
+      <c r="B65" t="s">
+        <v>91</v>
+      </c>
+      <c r="C65" t="s">
+        <v>92</v>
+      </c>
+      <c r="D65" s="3">
+        <v>46174</v>
+      </c>
+      <c r="E65" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F65">
+        <v>1132</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>508</v>
+      </c>
+      <c r="I65">
+        <v>18414</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>100000</v>
+      </c>
+      <c r="L65" t="s">
+        <v>60</v>
+      </c>
+      <c r="M65" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>45561.857662037037</v>
+      </c>
+      <c r="B66" t="s">
+        <v>93</v>
+      </c>
+      <c r="C66" t="s">
+        <v>94</v>
+      </c>
+      <c r="D66" s="3">
+        <v>15097</v>
+      </c>
+      <c r="E66" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F66">
+        <v>1132</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>508</v>
+      </c>
+      <c r="I66">
+        <v>27904</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>100000</v>
+      </c>
+      <c r="L66" t="s">
+        <v>60</v>
+      </c>
+      <c r="M66" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>45561.859363425923</v>
+      </c>
+      <c r="B67" t="s">
+        <v>95</v>
+      </c>
+      <c r="C67" t="s">
+        <v>96</v>
+      </c>
+      <c r="D67" s="3">
+        <v>29677</v>
+      </c>
+      <c r="E67" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F67">
+        <v>1132</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>508</v>
+      </c>
+      <c r="I67">
+        <v>13497</v>
+      </c>
+      <c r="J67">
+        <v>0</v>
+      </c>
+      <c r="K67">
+        <v>100000</v>
+      </c>
+      <c r="L67" t="s">
+        <v>60</v>
+      </c>
+      <c r="M67" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>45561.860983796294</v>
+      </c>
+      <c r="B68" t="s">
+        <v>97</v>
+      </c>
+      <c r="C68" t="s">
+        <v>98</v>
+      </c>
+      <c r="D68" s="3">
+        <v>27120</v>
+      </c>
+      <c r="E68" s="2">
+        <v>0.99</v>
+      </c>
+      <c r="F68">
+        <v>1120</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>505</v>
+      </c>
+      <c r="I68">
+        <v>13713</v>
+      </c>
+      <c r="J68">
+        <v>0</v>
+      </c>
+      <c r="K68">
+        <v>100000</v>
+      </c>
+      <c r="L68" t="s">
+        <v>60</v>
+      </c>
+      <c r="M68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>